<commit_message>
Be more informative in FilesNotFoundError exception in metadata; also new version of metadata for testing
</commit_message>
<xml_diff>
--- a/biogaz_libraries_metadata_sample.xlsx
+++ b/biogaz_libraries_metadata_sample.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="165">
   <si>
     <t>library_id</t>
   </si>
@@ -475,73 +475,64 @@
     <t>/seq/miSEQ/miSEQ_18th/bustard_0/Project_Diversity_Biogazownia/Sample_16S_BacV3V4_M_BH_06/</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_16st_1</t>
+    <t>GB_RNA_stress_16st_1</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_16st_1</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH5_1</t>
+    <t>GB_RNA_stress_pH5_1</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH5_1</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH7_1</t>
-  </si>
-  <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH7_1</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH9_1</t>
+    <t>GB_RNA_stress_pH9_1</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH9_1</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_16st_2</t>
+    <t>GB_RNA_stress_16st_2</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_16st_2</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH5_2</t>
+    <t>GB_RNA_stress_pH5_2</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH5_2</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH7_2</t>
-  </si>
-  <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH7_2</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH9_2</t>
+    <t>GB_RNA_stress_pH9_2</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH9_2</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_16st_3</t>
+    <t>GB_RNA_stress_16st_3</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_16st_3</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH5_3</t>
+    <t>GB_RNA_stress_pH5_3</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH5_3</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH7_3</t>
-  </si>
-  <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH7_3</t>
   </si>
   <si>
-    <t>Sample_GB_RNA_stress_pH9_3</t>
+    <t>GB_RNA_stress_pH9_3</t>
   </si>
   <si>
     <t>/home/pszczesny/storage/20150921_web_interface_test/trans/Sample_GB_RNA_stress_pH9_3</t>
@@ -652,8 +643,8 @@
   </sheetPr>
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2833,10 +2824,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2844,10 +2835,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,10 +2846,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,10 +2857,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,10 +2868,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,10 +2879,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2899,10 +2890,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,10 +2901,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,10 +2912,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,10 +2923,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>